<commit_message>
correcao plano de teste
</commit_message>
<xml_diff>
--- a/PLANO DE TESTE-1-1.xlsx
+++ b/PLANO DE TESTE-1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Desktop\facens\teste\af-testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D21A7B40-A27E-4851-9322-CD36419199C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387D94EE-4650-40D0-ABC3-52E5F772BE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>PROJETO / SISTEMA</t>
   </si>
@@ -224,13 +224,19 @@
   </si>
   <si>
     <t>AC2</t>
+  </si>
+  <si>
+    <t>Statement st = conn.createStatement();</t>
+  </si>
+  <si>
+    <t>Connection conn = conectarDB(); pode retornar null, e o "tratamento" existente é a execução dentro do bloco try-catch, o que não configura boa prática, ainda mais com o bloco catch vazio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +298,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -519,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -631,6 +644,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1245,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,18 +1374,22 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
@@ -1428,5 +1448,6 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>